<commit_message>
Update of GINF2 list
</commit_message>
<xml_diff>
--- a/resources/GINF2/liste.xlsx
+++ b/resources/GINF2/liste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F5D0F4E-6781-4600-B9E8-23CF95F6EAE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCECB584-8EF9-419D-937B-DC7AD4D912FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{889BF72A-A84D-4ADE-8707-2DE0EE261D62}"/>
+    <workbookView xWindow="4065" yWindow="3195" windowWidth="15375" windowHeight="8325" xr2:uid="{889BF72A-A84D-4ADE-8707-2DE0EE261D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="93">
   <si>
     <t xml:space="preserve">Nom </t>
   </si>
@@ -34,6 +34,276 @@
   </si>
   <si>
     <t>CIN</t>
+  </si>
+  <si>
+    <t>Achabar</t>
+  </si>
+  <si>
+    <t>Adnane</t>
+  </si>
+  <si>
+    <t>Adraoui</t>
+  </si>
+  <si>
+    <t>Khaoula</t>
+  </si>
+  <si>
+    <t>Ahmadoun</t>
+  </si>
+  <si>
+    <t>Mohamed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ameziane </t>
+  </si>
+  <si>
+    <t>Chaimae</t>
+  </si>
+  <si>
+    <t>Bentaher</t>
+  </si>
+  <si>
+    <t>Bouhal</t>
+  </si>
+  <si>
+    <t>Basma</t>
+  </si>
+  <si>
+    <t>Bouzekraoui</t>
+  </si>
+  <si>
+    <t>Asmae</t>
+  </si>
+  <si>
+    <t>Benabdellah</t>
+  </si>
+  <si>
+    <t>El Azizi</t>
+  </si>
+  <si>
+    <t>Hamza</t>
+  </si>
+  <si>
+    <t>El Bourkadi</t>
+  </si>
+  <si>
+    <t>Oussama</t>
+  </si>
+  <si>
+    <t>El Asli</t>
+  </si>
+  <si>
+    <t>Mariam</t>
+  </si>
+  <si>
+    <t>El mansori</t>
+  </si>
+  <si>
+    <t>Issam</t>
+  </si>
+  <si>
+    <t>El mamaoune</t>
+  </si>
+  <si>
+    <t>Mouad</t>
+  </si>
+  <si>
+    <t>Elkasmi</t>
+  </si>
+  <si>
+    <t>Fatima Zhora</t>
+  </si>
+  <si>
+    <t>El Hassani</t>
+  </si>
+  <si>
+    <t>Sokayna</t>
+  </si>
+  <si>
+    <t>Insaf</t>
+  </si>
+  <si>
+    <t>Jaadar</t>
+  </si>
+  <si>
+    <t>Sami</t>
+  </si>
+  <si>
+    <t>Kaadiri</t>
+  </si>
+  <si>
+    <t>Abdelatif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noufel </t>
+  </si>
+  <si>
+    <t>Salima</t>
+  </si>
+  <si>
+    <t>Ngan</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Sahel</t>
+  </si>
+  <si>
+    <t>Ikrame</t>
+  </si>
+  <si>
+    <t>Salmoun</t>
+  </si>
+  <si>
+    <t>Serrad</t>
+  </si>
+  <si>
+    <t>Hajar</t>
+  </si>
+  <si>
+    <t>Tatani</t>
+  </si>
+  <si>
+    <t>Herman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zalai </t>
+  </si>
+  <si>
+    <t>Yazid</t>
+  </si>
+  <si>
+    <t>Aissa</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Laidouni</t>
+  </si>
+  <si>
+    <t>Youssef</t>
+  </si>
+  <si>
+    <t>Echtioui</t>
+  </si>
+  <si>
+    <t>Salma</t>
+  </si>
+  <si>
+    <t>El Moustachir</t>
+  </si>
+  <si>
+    <t>Yassine</t>
+  </si>
+  <si>
+    <t>Mansour</t>
+  </si>
+  <si>
+    <t>El Mhedi</t>
+  </si>
+  <si>
+    <t>Jadar</t>
+  </si>
+  <si>
+    <t>Sahli</t>
+  </si>
+  <si>
+    <t>Kawtar</t>
+  </si>
+  <si>
+    <t>El Ouazani</t>
+  </si>
+  <si>
+    <t>Zohra</t>
+  </si>
+  <si>
+    <t>Maztaoui</t>
+  </si>
+  <si>
+    <t>Ilias</t>
+  </si>
+  <si>
+    <t>Bouabib</t>
+  </si>
+  <si>
+    <t>Iness</t>
+  </si>
+  <si>
+    <t>Kherraf</t>
+  </si>
+  <si>
+    <t>Taha</t>
+  </si>
+  <si>
+    <t>Essar-rhini</t>
+  </si>
+  <si>
+    <t>Souhaib</t>
+  </si>
+  <si>
+    <t>Falaki</t>
+  </si>
+  <si>
+    <t>Mchachti</t>
+  </si>
+  <si>
+    <t>Fezzazi</t>
+  </si>
+  <si>
+    <t>Mossaouir</t>
+  </si>
+  <si>
+    <t>Firdaous</t>
+  </si>
+  <si>
+    <t>Aymane</t>
+  </si>
+  <si>
+    <t>Dabdoubi</t>
+  </si>
+  <si>
+    <t>Chihi</t>
+  </si>
+  <si>
+    <t>Hasnae</t>
+  </si>
+  <si>
+    <t>El Aakkouchi</t>
+  </si>
+  <si>
+    <t>El Younssi</t>
+  </si>
+  <si>
+    <t>Mouna</t>
+  </si>
+  <si>
+    <t>Dachar</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Imane</t>
+  </si>
+  <si>
+    <t>Charfi</t>
+  </si>
+  <si>
+    <t>El Jettari</t>
+  </si>
+  <si>
+    <t>El Khayyat</t>
+  </si>
+  <si>
+    <t>Mohamed El Amine</t>
+  </si>
+  <si>
+    <t>Oumechtak</t>
+  </si>
+  <si>
+    <t>Rida</t>
   </si>
 </sst>
 </file>
@@ -385,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBF76A2F-C15E-4FF5-B172-1616349AC431}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,6 +674,398 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>